<commit_message>
Complete issue #35: Add comprehensive sectoral SCM analysis
- Corrected 'nearly doubling' wording (67% increase is accurate)
- Added Maule sectoral SCM analysis (construction and other sectors)
- Added inference diagnostics (RMSPE ratios, p-values) for sectoral SCM
- Quantified crowding-out in Canterbury (2pp decline in other sectors vs 4pp increase in construction)
- Created comprehensive sectoral appendix with tables and figures for both countries
- Added explicit conclusion on net stimulus vs sectoral reallocation
- Generated all sectoral figures: chile_scm_construccion.png, chile_scm_Other_Sectors.png, nz_scm_Construction.png, nz_scm_Other_Sectors.png
- Fixed pandas compatibility issue in nz_util.py

Co-authored-by: Diego Diaz <diegodiaz@uchicago.edu>
</commit_message>
<xml_diff>
--- a/article_assets/nz_sectorial.xlsx
+++ b/article_assets/nz_sectorial.xlsx
@@ -13,13 +13,14 @@
     <sheet name="Agriculture" sheetId="4" r:id="rId4"/>
     <sheet name="Manufacturing" sheetId="5" r:id="rId5"/>
     <sheet name="Rental," sheetId="6" r:id="rId6"/>
+    <sheet name="Inference" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
     <t>Synthetic Control</t>
   </si>
@@ -29,21 +30,46 @@
   <si>
     <t>Year</t>
   </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>RMSPE_Pre</t>
+  </si>
+  <si>
+    <t>RMSPE_Post</t>
+  </si>
+  <si>
+    <t>RMSPE_Ratio</t>
+  </si>
+  <si>
+    <t>Mean_Post_Gap</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Other_Sectors</t>
+  </si>
+  <si>
+    <t>Financial and Insurance Services</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Rental, Hiring and Real Estate Services</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -59,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -67,30 +93,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,264 +400,264 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>2000</v>
       </c>
       <c r="B2">
-        <v>4.898204692516823</v>
+        <v>4.909354875538632</v>
       </c>
       <c r="C2">
         <v>4.691903419910123</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2001</v>
       </c>
       <c r="B3">
-        <v>4.674806468146371</v>
+        <v>4.681860772777387</v>
       </c>
       <c r="C3">
         <v>4.668696534725242</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2002</v>
       </c>
       <c r="B4">
-        <v>4.783217411907941</v>
+        <v>4.791049753811859</v>
       </c>
       <c r="C4">
         <v>4.817567567567568</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>2003</v>
       </c>
       <c r="B5">
-        <v>5.128222217062095</v>
+        <v>5.139543440038089</v>
       </c>
       <c r="C5">
         <v>5.033557046979865</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>2004</v>
       </c>
       <c r="B6">
-        <v>5.344699086968487</v>
+        <v>5.34886721368235</v>
       </c>
       <c r="C6">
         <v>5.379746835443038</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>2005</v>
       </c>
       <c r="B7">
-        <v>6.207950290022656</v>
+        <v>6.205922490123703</v>
       </c>
       <c r="C7">
         <v>6.148572652777034</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>2006</v>
       </c>
       <c r="B8">
-        <v>5.779414134456607</v>
+        <v>5.784947119907189</v>
       </c>
       <c r="C8">
         <v>5.970452353150226</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>2007</v>
       </c>
       <c r="B9">
-        <v>6.128865198362155</v>
+        <v>6.143480909695239</v>
       </c>
       <c r="C9">
         <v>6.115056479672084</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>2008</v>
       </c>
       <c r="B10">
-        <v>6.391929230992209</v>
+        <v>6.400035322846863</v>
       </c>
       <c r="C10">
         <v>6.523373579231348</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>2009</v>
       </c>
       <c r="B11">
-        <v>6.186155356834866</v>
+        <v>6.191352450004326</v>
       </c>
       <c r="C11">
         <v>6.07488647073944</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>2010</v>
       </c>
       <c r="B12">
-        <v>6.187497419704215</v>
+        <v>6.191166133080032</v>
       </c>
       <c r="C12">
         <v>5.813177648040034</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>2011</v>
       </c>
       <c r="B13">
-        <v>5.836715012102111</v>
+        <v>5.841801154118497</v>
       </c>
       <c r="C13">
         <v>5.82281495594189</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>2012</v>
       </c>
       <c r="B14">
-        <v>5.466609754729451</v>
+        <v>5.477257431048647</v>
       </c>
       <c r="C14">
         <v>6.914873572747485</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>2013</v>
       </c>
       <c r="B15">
-        <v>5.728984083926886</v>
+        <v>5.72953994413719</v>
       </c>
       <c r="C15">
         <v>8.298755186721991</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>2014</v>
       </c>
       <c r="B16">
-        <v>5.532594065001518</v>
+        <v>5.522285612648909</v>
       </c>
       <c r="C16">
         <v>8.872620790629576</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>2015</v>
       </c>
       <c r="B17">
-        <v>5.767041291820732</v>
+        <v>5.759116819788894</v>
       </c>
       <c r="C17">
         <v>9.83616769451193</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>2016</v>
       </c>
       <c r="B18">
-        <v>5.952605510324477</v>
+        <v>5.943320960741827</v>
       </c>
       <c r="C18">
         <v>9.969214052879391</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>2017</v>
       </c>
       <c r="B19">
-        <v>6.18861648416128</v>
+        <v>6.179500522456502</v>
       </c>
       <c r="C19">
         <v>9.143342311746105</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>2018</v>
       </c>
       <c r="B20">
-        <v>6.542150153520724</v>
+        <v>6.530929923641208</v>
       </c>
       <c r="C20">
         <v>8.98361906838562</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>2019</v>
       </c>
       <c r="B21">
-        <v>6.805449958655214</v>
+        <v>6.794157231708999</v>
       </c>
       <c r="C21">
         <v>8.674308692586887</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>2020</v>
       </c>
       <c r="B22">
-        <v>7.365373290433119</v>
+        <v>7.362478398071418</v>
       </c>
       <c r="C22">
         <v>8.592227020357804</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>2021</v>
       </c>
       <c r="B23">
-        <v>7.5961460460051</v>
+        <v>7.586174354828828</v>
       </c>
       <c r="C23">
         <v>8.672113641443365</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>2022</v>
       </c>
       <c r="B24">
-        <v>7.264812909575749</v>
+        <v>7.246887571771938</v>
       </c>
       <c r="C24">
         <v>8.358154657693095</v>
@@ -669,264 +677,264 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>2000</v>
       </c>
       <c r="B2">
-        <v>70.03696382524441</v>
+        <v>70.03696071999781</v>
       </c>
       <c r="C2">
         <v>75.28372305583059</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2001</v>
       </c>
       <c r="B3">
-        <v>71.03745398447369</v>
+        <v>71.03745231059301</v>
       </c>
       <c r="C3">
         <v>76.01130926489778</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2002</v>
       </c>
       <c r="B4">
-        <v>71.56293202668304</v>
+        <v>71.56292968461145</v>
       </c>
       <c r="C4">
         <v>76.54729729729731</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>2003</v>
       </c>
       <c r="B5">
-        <v>70.36612353694393</v>
+        <v>70.36612088251015</v>
       </c>
       <c r="C5">
         <v>76.03520324173736</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>2004</v>
       </c>
       <c r="B6">
-        <v>70.96063331795395</v>
+        <v>70.96063091353383</v>
       </c>
       <c r="C6">
         <v>75.37505860290669</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>2005</v>
       </c>
       <c r="B7">
-        <v>69.91490456628054</v>
+        <v>69.91490152871764</v>
       </c>
       <c r="C7">
         <v>74.42022387660006</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>2006</v>
       </c>
       <c r="B8">
-        <v>69.16779397367897</v>
+        <v>69.16778917520644</v>
       </c>
       <c r="C8">
         <v>74.26003959993906</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>2007</v>
       </c>
       <c r="B9">
-        <v>67.91511881438288</v>
+        <v>67.9151126453994</v>
       </c>
       <c r="C9">
         <v>73.16143177160288</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>2008</v>
       </c>
       <c r="B10">
-        <v>67.25924107357879</v>
+        <v>67.25923112711487</v>
       </c>
       <c r="C10">
         <v>73.44655256291186</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>2009</v>
       </c>
       <c r="B11">
-        <v>66.91385178774337</v>
+        <v>66.91384245710941</v>
       </c>
       <c r="C11">
         <v>73.58409733527547</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>2010</v>
       </c>
       <c r="B12">
-        <v>67.60490067526793</v>
+        <v>67.60489218264939</v>
       </c>
       <c r="C12">
         <v>74.76647206005006</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>2011</v>
       </c>
       <c r="B13">
-        <v>67.02534209102274</v>
+        <v>67.02533444895845</v>
       </c>
       <c r="C13">
         <v>73.78740970072239</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>2012</v>
       </c>
       <c r="B14">
-        <v>67.10090626118622</v>
+        <v>67.10089822192366</v>
       </c>
       <c r="C14">
         <v>72.41210385499491</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>2013</v>
       </c>
       <c r="B15">
-        <v>66.63575308085453</v>
+        <v>66.63574525273724</v>
       </c>
       <c r="C15">
         <v>70.48529677070178</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>2014</v>
       </c>
       <c r="B16">
-        <v>67.86075361372302</v>
+        <v>67.86074708678451</v>
       </c>
       <c r="C16">
         <v>70.09598177972995</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>2015</v>
       </c>
       <c r="B17">
-        <v>67.31401274435625</v>
+        <v>67.31400499545701</v>
       </c>
       <c r="C17">
         <v>68.40465956519031</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>2016</v>
       </c>
       <c r="B18">
-        <v>67.04832254270292</v>
+        <v>67.0483170069154</v>
       </c>
       <c r="C18">
         <v>68.65568030906675</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>2017</v>
       </c>
       <c r="B19">
-        <v>67.01121493983312</v>
+        <v>67.01120955811074</v>
       </c>
       <c r="C19">
         <v>69.30846703361048</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>2018</v>
       </c>
       <c r="B20">
-        <v>66.39477062296865</v>
+        <v>66.39476429267414</v>
       </c>
       <c r="C20">
         <v>70.14363978304124</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>2019</v>
       </c>
       <c r="B21">
-        <v>66.37016773122434</v>
+        <v>66.37016209134727</v>
       </c>
       <c r="C21">
         <v>70.15693135232524</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>2020</v>
       </c>
       <c r="B22">
-        <v>66.53108008529991</v>
+        <v>66.5310739953849</v>
       </c>
       <c r="C22">
         <v>70.2134484885873</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>2021</v>
       </c>
       <c r="B23">
-        <v>67.53667505525389</v>
+        <v>67.53666946896473</v>
       </c>
       <c r="C23">
         <v>70.61613728363176</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>2022</v>
       </c>
       <c r="B24">
-        <v>67.94760332686536</v>
+        <v>67.94759804405861</v>
       </c>
       <c r="C24">
         <v>70.5941201882631</v>
@@ -946,264 +954,264 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>2000</v>
       </c>
       <c r="B2">
-        <v>3.004069781393836</v>
+        <v>3.00992281240767</v>
       </c>
       <c r="C2">
         <v>2.825805468809506</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2001</v>
       </c>
       <c r="B3">
-        <v>3.102896503480782</v>
+        <v>3.119219188670747</v>
       </c>
       <c r="C3">
         <v>2.83456575322604</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2002</v>
       </c>
       <c r="B4">
-        <v>3.159565842375182</v>
+        <v>3.20044566148106</v>
       </c>
       <c r="C4">
         <v>3.060810810810811</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>2003</v>
       </c>
       <c r="B5">
-        <v>3.345842973021196</v>
+        <v>3.350867203753796</v>
       </c>
       <c r="C5">
         <v>3.362036216284666</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>2004</v>
       </c>
       <c r="B6">
-        <v>3.57243143185658</v>
+        <v>3.581513195913283</v>
       </c>
       <c r="C6">
         <v>3.656821378340366</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>2005</v>
       </c>
       <c r="B7">
-        <v>3.627857576965845</v>
+        <v>3.611754875812044</v>
       </c>
       <c r="C7">
         <v>3.840179958223984</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>2006</v>
       </c>
       <c r="B8">
-        <v>3.610118876188946</v>
+        <v>3.592473108080242</v>
       </c>
       <c r="C8">
         <v>3.690917398588617</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>2007</v>
       </c>
       <c r="B9">
-        <v>3.444686850067099</v>
+        <v>3.427637427889325</v>
       </c>
       <c r="C9">
         <v>3.512701968447643</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>2008</v>
       </c>
       <c r="B10">
-        <v>3.329302952436769</v>
+        <v>3.287682421441319</v>
       </c>
       <c r="C10">
         <v>3.312546990402901</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>2009</v>
       </c>
       <c r="B11">
-        <v>3.738906222647267</v>
+        <v>3.670919484560697</v>
       </c>
       <c r="C11">
         <v>3.654356953131694</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>2010</v>
       </c>
       <c r="B12">
-        <v>4.312115682785975</v>
+        <v>4.311852415028941</v>
       </c>
       <c r="C12">
         <v>4.065888240200167</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>2011</v>
       </c>
       <c r="B13">
-        <v>3.770272774821767</v>
+        <v>3.718027642844674</v>
       </c>
       <c r="C13">
         <v>3.433357148527427</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>2012</v>
       </c>
       <c r="B14">
-        <v>3.975862800033791</v>
+        <v>3.892211620548045</v>
       </c>
       <c r="C14">
         <v>2.999585484417983</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>2013</v>
       </c>
       <c r="B15">
-        <v>3.952219706960987</v>
+        <v>3.874455470866506</v>
       </c>
       <c r="C15">
         <v>3.146310662096337</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>2014</v>
       </c>
       <c r="B16">
-        <v>4.016074262671255</v>
+        <v>3.939770242643672</v>
       </c>
       <c r="C16">
         <v>3.237351553603384</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>2015</v>
       </c>
       <c r="B17">
-        <v>4.30415795521462</v>
+        <v>4.216545727569942</v>
       </c>
       <c r="C17">
         <v>3.28599015760294</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>2016</v>
       </c>
       <c r="B18">
-        <v>3.998006420060119</v>
+        <v>3.968085253486091</v>
       </c>
       <c r="C18">
         <v>2.716407098877218</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>2017</v>
       </c>
       <c r="B19">
-        <v>3.994292098945303</v>
+        <v>3.985776811500933</v>
       </c>
       <c r="C19">
         <v>2.415388218760979</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>2018</v>
       </c>
       <c r="B20">
-        <v>4.09796822323016</v>
+        <v>4.219435331686264</v>
       </c>
       <c r="C20">
         <v>3.109923955408978</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>2019</v>
       </c>
       <c r="B21">
-        <v>4.076536620541284</v>
+        <v>4.137767791437408</v>
       </c>
       <c r="C21">
         <v>3.459801028801211</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>2020</v>
       </c>
       <c r="B22">
-        <v>3.961750843529029</v>
+        <v>3.979826737113193</v>
       </c>
       <c r="C22">
         <v>3.195558297347317</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>2021</v>
       </c>
       <c r="B23">
-        <v>4.183596295985767</v>
+        <v>4.19878336860629</v>
       </c>
       <c r="C23">
         <v>3.38738917724191</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>2022</v>
       </c>
       <c r="B24">
-        <v>4.290435781227723</v>
+        <v>4.290798380046681</v>
       </c>
       <c r="C24">
         <v>3.66976649007526</v>
@@ -1223,264 +1231,264 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>2000</v>
       </c>
       <c r="B2">
-        <v>5.299514828675615</v>
+        <v>5.318282310693759</v>
       </c>
       <c r="C2">
         <v>5.567826947977759</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2001</v>
       </c>
       <c r="B3">
-        <v>6.776827752118433</v>
+        <v>6.80438705138756</v>
       </c>
       <c r="C3">
         <v>7.133536320139192</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2002</v>
       </c>
       <c r="B4">
-        <v>7.095467255295068</v>
+        <v>7.126512227482343</v>
       </c>
       <c r="C4">
         <v>7.290540540540541</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>2003</v>
       </c>
       <c r="B5">
-        <v>5.292975915973049</v>
+        <v>5.307523136718197</v>
       </c>
       <c r="C5">
         <v>5.628719767000127</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>2004</v>
       </c>
       <c r="B6">
-        <v>5.718932039965936</v>
+        <v>5.719130016857253</v>
       </c>
       <c r="C6">
         <v>5.29184247538678</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>2005</v>
       </c>
       <c r="B7">
-        <v>5.242677825195063</v>
+        <v>5.249898607650811</v>
       </c>
       <c r="C7">
         <v>4.997054255262171</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>2006</v>
       </c>
       <c r="B8">
-        <v>4.543163425968809</v>
+        <v>4.541407462255786</v>
       </c>
       <c r="C8">
         <v>4.046301467228512</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>2007</v>
       </c>
       <c r="B9">
-        <v>4.624484486389573</v>
+        <v>4.63281278389741</v>
       </c>
       <c r="C9">
         <v>4.451646727991992</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>2008</v>
       </c>
       <c r="B10">
-        <v>5.492370132122408</v>
+        <v>5.524760988745911</v>
       </c>
       <c r="C10">
         <v>6.364159037636549</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>2009</v>
       </c>
       <c r="B11">
-        <v>4.473771270475509</v>
+        <v>4.495523460456369</v>
       </c>
       <c r="C11">
         <v>5.098106417616314</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>2010</v>
       </c>
       <c r="B12">
-        <v>5.051141420235953</v>
+        <v>5.094819016888716</v>
       </c>
       <c r="C12">
         <v>6.609674728940784</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>2011</v>
       </c>
       <c r="B13">
-        <v>5.704510279195977</v>
+        <v>5.760159237561744</v>
       </c>
       <c r="C13">
         <v>7.402556164166072</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>2012</v>
       </c>
       <c r="B14">
-        <v>5.645595190960682</v>
+        <v>5.699048411927259</v>
       </c>
       <c r="C14">
         <v>7.306779213927723</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>2013</v>
       </c>
       <c r="B15">
-        <v>4.82187400900714</v>
+        <v>4.862708248163462</v>
       </c>
       <c r="C15">
         <v>6.126646220458236</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>2014</v>
       </c>
       <c r="B16">
-        <v>6.349584750134787</v>
+        <v>6.403922498250678</v>
       </c>
       <c r="C16">
         <v>8.166585326175371</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>2015</v>
       </c>
       <c r="B17">
-        <v>4.446999051899764</v>
+        <v>4.464821979233463</v>
       </c>
       <c r="C17">
         <v>4.656450507693267</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>2016</v>
       </c>
       <c r="B18">
-        <v>4.100350266420389</v>
+        <v>4.101512155680004</v>
       </c>
       <c r="C18">
         <v>4.122902330073645</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>2017</v>
       </c>
       <c r="B19">
-        <v>5.014757199881236</v>
+        <v>5.032137675800048</v>
       </c>
       <c r="C19">
         <v>6.118983487527814</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>2018</v>
       </c>
       <c r="B20">
-        <v>5.218594305436418</v>
+        <v>5.244192295436321</v>
       </c>
       <c r="C20">
         <v>6.604159284799259</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>2019</v>
       </c>
       <c r="B21">
-        <v>4.85626582320203</v>
+        <v>4.882554067475919</v>
       </c>
       <c r="C21">
         <v>6.334699845940936</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>2020</v>
       </c>
       <c r="B22">
-        <v>5.003620590755669</v>
+        <v>5.034262621290559</v>
       </c>
       <c r="C22">
         <v>6.706971005552129</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>2021</v>
       </c>
       <c r="B23">
-        <v>4.978797510951583</v>
+        <v>5.015181403765334</v>
       </c>
       <c r="C23">
         <v>7.147291827054411</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>2022</v>
       </c>
       <c r="B24">
-        <v>5.059789117811563</v>
+        <v>5.100594466202272</v>
       </c>
       <c r="C24">
         <v>7.416839089606876</v>
@@ -1500,264 +1508,264 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>2000</v>
       </c>
       <c r="B2">
-        <v>15.53357935066167</v>
+        <v>15.53371666517171</v>
       </c>
       <c r="C2">
         <v>16.68063066494021</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2001</v>
       </c>
       <c r="B3">
-        <v>15.5343499259491</v>
+        <v>15.53530257137981</v>
       </c>
       <c r="C3">
         <v>16.10120342177758</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2002</v>
       </c>
       <c r="B4">
-        <v>15.10977488557459</v>
+        <v>15.11131679546708</v>
       </c>
       <c r="C4">
         <v>15.87162162162162</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>2003</v>
       </c>
       <c r="B5">
-        <v>15.23592400619139</v>
+        <v>15.236606742019</v>
       </c>
       <c r="C5">
         <v>16.27833354438394</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>2004</v>
       </c>
       <c r="B6">
-        <v>14.04862706114345</v>
+        <v>14.04929705430803</v>
       </c>
       <c r="C6">
         <v>15.57665260196906</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>2005</v>
       </c>
       <c r="B7">
-        <v>13.71515658377637</v>
+        <v>13.71605510353847</v>
       </c>
       <c r="C7">
         <v>15.33394033527931</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>2006</v>
       </c>
       <c r="B8">
-        <v>13.38316300824044</v>
+        <v>13.3846279909916</v>
       </c>
       <c r="C8">
         <v>15.14951515459207</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>2007</v>
       </c>
       <c r="B9">
-        <v>12.86480007168883</v>
+        <v>12.8659644013366</v>
       </c>
       <c r="C9">
         <v>14.00791192030885</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>2008</v>
       </c>
       <c r="B10">
-        <v>12.45576065584176</v>
+        <v>12.45645853700634</v>
       </c>
       <c r="C10">
         <v>13.0865507938614</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>2009</v>
       </c>
       <c r="B11">
-        <v>11.90105021792679</v>
+        <v>11.90194394046013</v>
       </c>
       <c r="C11">
         <v>13.64921600548368</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>2010</v>
       </c>
       <c r="B12">
-        <v>10.89303100021529</v>
+        <v>10.89402385347335</v>
       </c>
       <c r="C12">
         <v>12.65638031693078</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>2011</v>
       </c>
       <c r="B13">
-        <v>10.96482383023019</v>
+        <v>10.96630295927072</v>
       </c>
       <c r="C13">
         <v>12.52282289433992</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>2012</v>
       </c>
       <c r="B14">
-        <v>10.95829516984418</v>
+        <v>10.95956756856186</v>
       </c>
       <c r="C14">
         <v>12.24705128688247</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>2013</v>
       </c>
       <c r="B15">
-        <v>10.55051276171642</v>
+        <v>10.55122509245605</v>
       </c>
       <c r="C15">
         <v>11.70485296770702</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>2014</v>
       </c>
       <c r="B16">
-        <v>10.08663747064423</v>
+        <v>10.08793780686504</v>
       </c>
       <c r="C16">
         <v>10.63282902228729</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>2015</v>
       </c>
       <c r="B17">
-        <v>10.73731389233262</v>
+        <v>10.73871690942542</v>
       </c>
       <c r="C17">
         <v>11.58661932349094</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>2016</v>
       </c>
       <c r="B18">
-        <v>10.92253045345875</v>
+        <v>10.92449051656184</v>
       </c>
       <c r="C18">
         <v>12.38379814077025</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>2017</v>
       </c>
       <c r="B19">
-        <v>10.05189294088914</v>
+        <v>10.05351042074362</v>
       </c>
       <c r="C19">
         <v>10.99074833118632</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>2018</v>
       </c>
       <c r="B20">
-        <v>10.03696673781738</v>
+        <v>10.03859794262687</v>
       </c>
       <c r="C20">
         <v>11.14230423287634</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>2019</v>
       </c>
       <c r="B21">
-        <v>9.694630505960488</v>
+        <v>9.696276141096854</v>
       </c>
       <c r="C21">
         <v>10.71624409222655</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>2020</v>
       </c>
       <c r="B22">
-        <v>9.394170527868987</v>
+        <v>9.395790122008396</v>
       </c>
       <c r="C22">
         <v>10.78346699568168</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>2021</v>
       </c>
       <c r="B23">
-        <v>9.024226407952517</v>
+        <v>9.025266848704593</v>
       </c>
       <c r="C23">
         <v>10.38567561526808</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>2022</v>
       </c>
       <c r="B24">
-        <v>8.751488427612253</v>
+        <v>8.752646223152736</v>
       </c>
       <c r="C24">
         <v>9.338123280507492</v>
@@ -1777,267 +1785,399 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>2000</v>
       </c>
       <c r="B2">
-        <v>5.673037396646611</v>
+        <v>5.621317299995464</v>
       </c>
       <c r="C2">
         <v>5.423109147688324</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2001</v>
       </c>
       <c r="B3">
-        <v>5.593793285639577</v>
+        <v>5.564318811431222</v>
       </c>
       <c r="C3">
         <v>5.437146585471944</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>2002</v>
       </c>
       <c r="B4">
-        <v>5.474693908353848</v>
+        <v>5.467196411875582</v>
       </c>
       <c r="C4">
         <v>5.506756756756757</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>2003</v>
       </c>
       <c r="B5">
-        <v>5.778535694016725</v>
+        <v>5.799167296374685</v>
       </c>
       <c r="C5">
         <v>5.774344687856148</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>2004</v>
       </c>
       <c r="B6">
-        <v>6.008938640744006</v>
+        <v>6.017210646691405</v>
       </c>
       <c r="C6">
         <v>6.03609939052977</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>2005</v>
       </c>
       <c r="B7">
-        <v>6.175958500405886</v>
+        <v>6.198518981985159</v>
       </c>
       <c r="C7">
         <v>6.121793155160409</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>2006</v>
       </c>
       <c r="B8">
-        <v>6.39274370757945</v>
+        <v>6.378247598254934</v>
       </c>
       <c r="C8">
         <v>6.655835914098594</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>2007</v>
       </c>
       <c r="B9">
-        <v>6.528794543803874</v>
+        <v>6.523318826965772</v>
       </c>
       <c r="C9">
         <v>6.748963347790858</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>2008</v>
       </c>
       <c r="B10">
-        <v>6.148810257003924</v>
+        <v>6.176825746001917</v>
       </c>
       <c r="C10">
         <v>5.970545309804963</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>2009</v>
       </c>
       <c r="B11">
-        <v>6.669231872638262</v>
+        <v>6.689039777759969</v>
       </c>
       <c r="C11">
         <v>6.383343329620426</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1">
+      <c r="A12">
         <v>2010</v>
       </c>
       <c r="B12">
-        <v>7.222379152433571</v>
+        <v>7.261371899193909</v>
       </c>
       <c r="C12">
         <v>7.043369474562135</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="1">
+      <c r="A13">
         <v>2011</v>
       </c>
       <c r="B13">
-        <v>7.04124107254068</v>
+        <v>7.04854462044021</v>
       </c>
       <c r="C13">
         <v>6.961975073430182</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="1">
+      <c r="A14">
         <v>2012</v>
       </c>
       <c r="B14">
-        <v>7.197729460763427</v>
+        <v>7.197291111761587</v>
       </c>
       <c r="C14">
         <v>7.144741304593587</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="1">
+      <c r="A15">
         <v>2013</v>
       </c>
       <c r="B15">
-        <v>7.254549581416198</v>
+        <v>7.25880297214124</v>
       </c>
       <c r="C15">
         <v>7.007035901136568</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1">
+      <c r="A16">
         <v>2014</v>
       </c>
       <c r="B16">
-        <v>7.107803631144457</v>
+        <v>7.109814302637266</v>
       </c>
       <c r="C16">
         <v>7.216528387831462</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1">
+      <c r="A17">
         <v>2015</v>
       </c>
       <c r="B17">
-        <v>6.982278432981371</v>
+        <v>6.974612893596587</v>
       </c>
       <c r="C17">
         <v>7.020494611599077</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1">
+      <c r="A18">
         <v>2016</v>
       </c>
       <c r="B18">
-        <v>7.119168227401867</v>
+        <v>7.11063907522167</v>
       </c>
       <c r="C18">
         <v>6.818181818181817</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1">
+      <c r="A19">
         <v>2017</v>
       </c>
       <c r="B19">
-        <v>7.245051553077762</v>
+        <v>7.284064222783096</v>
       </c>
       <c r="C19">
         <v>6.994378732872701</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1">
+      <c r="A20">
         <v>2018</v>
       </c>
       <c r="B20">
-        <v>6.895792361090557</v>
+        <v>6.964782526682914</v>
       </c>
       <c r="C20">
         <v>6.609610509962113</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1">
+      <c r="A21">
         <v>2019</v>
       </c>
       <c r="B21">
-        <v>7.125340059673357</v>
+        <v>7.173406836040595</v>
       </c>
       <c r="C21">
         <v>6.825599916442542</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>2020</v>
       </c>
       <c r="B22">
-        <v>7.302343063833544</v>
+        <v>7.368357866644308</v>
       </c>
       <c r="C22">
         <v>6.679827267119062</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1">
+      <c r="A23">
         <v>2021</v>
       </c>
       <c r="B23">
-        <v>7.576384217657166</v>
+        <v>7.64478579410545</v>
       </c>
       <c r="C23">
         <v>6.777261777634291</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1">
+      <c r="A24">
         <v>2022</v>
       </c>
       <c r="B24">
-        <v>7.324369991899349</v>
+        <v>7.372003563562762</v>
       </c>
       <c r="C24">
         <v>6.643777995043314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>0.1568176074244797</v>
+      </c>
+      <c r="C2">
+        <v>2.499739061241317</v>
+      </c>
+      <c r="D2">
+        <v>15.94042341479507</v>
+      </c>
+      <c r="E2">
+        <v>2.180396810056857</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>5.531345688477642</v>
+      </c>
+      <c r="C3">
+        <v>3.66561950609198</v>
+      </c>
+      <c r="D3">
+        <v>0.6626994067154109</v>
+      </c>
+      <c r="E3">
+        <v>3.341445970545716</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>0.1568777600068354</v>
+      </c>
+      <c r="C4">
+        <v>0.9196888216176277</v>
+      </c>
+      <c r="D4">
+        <v>5.862455083356336</v>
+      </c>
+      <c r="E4">
+        <v>-0.8637212587990629</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0.6170032752778043</v>
+      </c>
+      <c r="C5">
+        <v>1.524037215625142</v>
+      </c>
+      <c r="D5">
+        <v>2.470063412449387</v>
+      </c>
+      <c r="E5">
+        <v>1.375814103515723</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1.321982956458023</v>
+      </c>
+      <c r="C6">
+        <v>1.147922369255937</v>
+      </c>
+      <c r="D6">
+        <v>0.8683337131149976</v>
+      </c>
+      <c r="E6">
+        <v>1.103683969312528</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>0.1847312011354326</v>
+      </c>
+      <c r="C7">
+        <v>0.4340397431970666</v>
+      </c>
+      <c r="D7">
+        <v>2.349574628050285</v>
+      </c>
+      <c r="E7">
+        <v>-0.3173077074809139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>